<commit_message>
aggiunto test in statistiche.xlsx
</commit_message>
<xml_diff>
--- a/statistiche/statistiche.xlsx
+++ b/statistiche/statistiche.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>CICLICHE</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>tutti i dati sono da intendersi in MEDIA</t>
+  </si>
+  <si>
+    <t>Test su grafi completi</t>
+  </si>
+  <si>
+    <t>k5</t>
+  </si>
+  <si>
+    <t>k7</t>
+  </si>
+  <si>
+    <t>k10</t>
   </si>
 </sst>
 </file>
@@ -169,6 +181,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -614,6 +627,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -731,6 +745,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -811,6 +826,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1433,6 +1449,708 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Tempo vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> dimensione CP-Net</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$D$93</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Backtracking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio1!$B$94:$B$96</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>k5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>k7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>k10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$D$94:$D$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2129999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$93</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B + FC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio1!$B$94:$B$96</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>k5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>k7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>k10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$E$94:$E$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.12E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6722999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$F$93</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B + AC3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Foglio1!$B$94:$B$96</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>k5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>k7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>k10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$F$94:$F$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9669999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1986506224"/>
+        <c:axId val="1986499696"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Foglio1!$C$93</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Foglio1!$B$94:$B$96</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>k5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>k7</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>k10</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Foglio1!$C$94:$C$96</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1986506224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Dimensione</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1986499696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1986499696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Tempo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1986506224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -1478,6 +2196,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1916,6 +2635,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2036,6 +2756,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2110,6 +2831,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6669,6 +7391,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8021,6 +8783,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -12400,6 +13665,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>117156</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12690,10 +13985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13415,7 +14710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C81">
         <v>50</v>
       </c>
@@ -13423,7 +14718,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>50</v>
       </c>
@@ -13434,7 +14729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C84">
         <v>10</v>
       </c>
@@ -13442,7 +14737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85">
         <v>15</v>
@@ -13451,7 +14746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C86">
         <v>30</v>
       </c>
@@ -13459,7 +14754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C87">
         <v>50</v>
       </c>
@@ -13467,9 +14762,65 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E94">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F94">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95">
+        <v>0.1227</v>
+      </c>
+      <c r="E95">
+        <v>0.1236</v>
+      </c>
+      <c r="F95">
+        <v>0.14849999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96">
+        <v>8.2129999999999992</v>
+      </c>
+      <c r="E96">
+        <v>7.6722999999999999</v>
+      </c>
+      <c r="F96">
+        <v>7.9669999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>